<commit_message>
more edits to readme, visuals
</commit_message>
<xml_diff>
--- a/proposal/capstone_1_proposal_example.xlsx
+++ b/proposal/capstone_1_proposal_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiffd/Documents/galvanize/capstone_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiffd/Documents/galvanize/rec_demographics/proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630E6B43-1F70-4249-8C2A-DC2A9BDF7416}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65D9F36-3035-1A4E-9854-D09DF432FDF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4160" yWindow="2420" windowWidth="25840" windowHeight="16940" xr2:uid="{3705DA75-8CC0-DD49-B4A6-1D926701FBC6}"/>
+    <workbookView xWindow="27040" yWindow="-17120" windowWidth="32700" windowHeight="17120" xr2:uid="{3705DA75-8CC0-DD49-B4A6-1D926701FBC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>HistoricalReservationID</t>
   </si>
@@ -115,13 +115,28 @@
   </si>
   <si>
     <t>[32344, 92064, 98006, 48118]</t>
+  </si>
+  <si>
+    <t>reservations.csv</t>
+  </si>
+  <si>
+    <t>reservation.csv</t>
+  </si>
+  <si>
+    <t>census api</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Data Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +146,15 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,12 +200,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +525,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +536,7 @@
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="29.6640625" customWidth="1"/>
-    <col min="15" max="15" width="22.5" customWidth="1"/>
+    <col min="15" max="15" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -608,111 +634,91 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2976269875</v>
-      </c>
-      <c r="B3" s="1">
-        <v>251937</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-135.31388888888799</v>
-      </c>
-      <c r="F3" s="1">
-        <v>59.4583333333333</v>
-      </c>
-      <c r="G3" s="2">
-        <v>92064</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2976269875</v>
-      </c>
-      <c r="B4" s="1">
-        <v>251937</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>-135.31388888888799</v>
-      </c>
-      <c r="F4" s="1">
-        <v>59.4583333333333</v>
-      </c>
-      <c r="G4" s="2">
-        <v>98006</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2976269875</v>
-      </c>
-      <c r="B5" s="1">
-        <v>251937</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-135.31388888888799</v>
-      </c>
-      <c r="F5" s="1">
-        <v>59.4583333333333</v>
-      </c>
-      <c r="G5" s="2">
-        <v>48118</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>